<commit_message>
write up the error
</commit_message>
<xml_diff>
--- a/Results/Model_Analysis.xlsx
+++ b/Results/Model_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Desktop\01Autonomous_Vehicles_Research\00Thesis\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9468A9B5-D8F8-42D0-8C22-8FF2DE9A65DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1C4803-2E2E-4B58-9B77-C144685AA569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -496,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,42 +635,17 @@
       <c r="P2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="2">
-        <f>E5</f>
-        <v>367.18956679377101</v>
-      </c>
-      <c r="R2" s="2">
-        <f t="shared" ref="R2:Y2" si="0">F5</f>
-        <v>0.6556492625164988</v>
-      </c>
-      <c r="S2" s="2">
-        <f t="shared" si="0"/>
-        <v>0.62945579912498928</v>
-      </c>
-      <c r="T2" s="2">
-        <f t="shared" si="0"/>
-        <v>0.55495181256883397</v>
-      </c>
-      <c r="U2" s="2">
-        <f t="shared" si="0"/>
-        <v>25.547793618574236</v>
-      </c>
-      <c r="V2" s="2">
-        <f t="shared" si="0"/>
-        <v>0.11070375128271874</v>
-      </c>
-      <c r="W2" s="2">
-        <f t="shared" si="0"/>
-        <v>384.79837399486041</v>
-      </c>
-      <c r="X2" s="2">
-        <f t="shared" si="0"/>
-        <v>0.77770651090318077</v>
-      </c>
-      <c r="Y2" s="2">
-        <f t="shared" si="0"/>
-        <v>367.18956679377101</v>
-      </c>
+      <c r="Q2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -715,42 +693,17 @@
       <c r="P3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="2">
-        <f>E10</f>
-        <v>214.71557153383665</v>
-      </c>
-      <c r="R3" s="2">
-        <f t="shared" ref="R3:Y3" si="1">F10</f>
-        <v>0.28003990870250622</v>
-      </c>
-      <c r="S3" s="2">
-        <f t="shared" si="1"/>
-        <v>0.47263579594587402</v>
-      </c>
-      <c r="T3" s="2">
-        <f t="shared" si="1"/>
-        <v>0.36327940323608904</v>
-      </c>
-      <c r="U3" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4575641553764784</v>
-      </c>
-      <c r="V3" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16783744476480314</v>
-      </c>
-      <c r="W3" s="2">
-        <f t="shared" si="1"/>
-        <v>119.54853129157205</v>
-      </c>
-      <c r="X3" s="2">
-        <f t="shared" si="1"/>
-        <v>0.32006144316351964</v>
-      </c>
-      <c r="Y3" s="2">
-        <f t="shared" si="1"/>
-        <v>214.71557153383665</v>
-      </c>
+      <c r="Q3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -798,42 +751,17 @@
       <c r="P4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="2">
-        <f>E16</f>
-        <v>107.54472776739135</v>
-      </c>
-      <c r="R4" s="2">
-        <f t="shared" ref="R4:Y4" si="2">F16</f>
-        <v>18.990594140551121</v>
-      </c>
-      <c r="S4" s="2">
-        <f t="shared" si="2"/>
-        <v>2.2569177029583769</v>
-      </c>
-      <c r="T4" s="2">
-        <f t="shared" si="2"/>
-        <v>0.5560004238669457</v>
-      </c>
-      <c r="U4" s="2">
-        <f t="shared" si="2"/>
-        <v>21.771239342500404</v>
-      </c>
-      <c r="V4" s="2">
-        <f t="shared" si="2"/>
-        <v>9.2366635485227333E-2</v>
-      </c>
-      <c r="W4" s="2">
-        <f t="shared" si="2"/>
-        <v>4043.3728961514335</v>
-      </c>
-      <c r="X4" s="2">
-        <f t="shared" si="2"/>
-        <v>0.68212620583395711</v>
-      </c>
-      <c r="Y4" s="2">
-        <f t="shared" si="2"/>
-        <v>107.54472776739135</v>
-      </c>
+      <c r="Q4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -851,31 +779,31 @@
         <v>0.6556492625164988</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:M5" si="3">AVERAGE(G2:G4)</f>
+        <f t="shared" ref="G5:M5" si="0">AVERAGE(G2:G4)</f>
         <v>0.62945579912498928</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.55495181256883397</v>
       </c>
       <c r="I5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>25.547793618574236</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.11070375128271874</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>384.79837399486041</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.77770651090318077</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>367.18956679377101</v>
       </c>
       <c r="O5" s="2" t="s">
@@ -884,42 +812,17 @@
       <c r="P5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="2">
-        <f>E21</f>
-        <v>294.83922401114938</v>
-      </c>
-      <c r="R5" s="2">
-        <f t="shared" ref="R5:Y5" si="4">F21</f>
-        <v>0.40268563150320075</v>
-      </c>
-      <c r="S5" s="2">
-        <f t="shared" si="4"/>
-        <v>0.5099631232466697</v>
-      </c>
-      <c r="T5" s="2">
-        <f t="shared" si="4"/>
-        <v>0.42850104887735235</v>
-      </c>
-      <c r="U5" s="2">
-        <f t="shared" si="4"/>
-        <v>23.365672473199567</v>
-      </c>
-      <c r="V5" s="2">
-        <f t="shared" si="4"/>
-        <v>8.8298729960432434E-2</v>
-      </c>
-      <c r="W5" s="2">
-        <f t="shared" si="4"/>
-        <v>244.90157111474659</v>
-      </c>
-      <c r="X5" s="2">
-        <f t="shared" si="4"/>
-        <v>0.86444195165420956</v>
-      </c>
-      <c r="Y5" s="2">
-        <f t="shared" si="4"/>
-        <v>294.83922401114938</v>
-      </c>
+      <c r="Q5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -941,42 +844,17 @@
       <c r="P6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="2">
-        <f>E26</f>
-        <v>239.838588937032</v>
-      </c>
-      <c r="R6" s="2">
-        <f t="shared" ref="R6:Y6" si="5">F26</f>
-        <v>0.54725963738798844</v>
-      </c>
-      <c r="S6" s="2">
-        <f t="shared" si="5"/>
-        <v>0.605114766793307</v>
-      </c>
-      <c r="T6" s="2">
-        <f t="shared" si="5"/>
-        <v>0.45106143856569797</v>
-      </c>
-      <c r="U6" s="2">
-        <f t="shared" si="5"/>
-        <v>1.7850433305725264</v>
-      </c>
-      <c r="V6" s="2">
-        <f t="shared" si="5"/>
-        <v>0.23020885798238935</v>
-      </c>
-      <c r="W6" s="2">
-        <f t="shared" si="5"/>
-        <v>196.60128855458296</v>
-      </c>
-      <c r="X6" s="2">
-        <f t="shared" si="5"/>
-        <v>-0.47296155363793796</v>
-      </c>
-      <c r="Y6" s="2">
-        <f t="shared" si="5"/>
-        <v>239.838588937032</v>
-      </c>
+      <c r="Q6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1024,42 +902,17 @@
       <c r="P7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="2">
-        <f>E32</f>
-        <v>123.31900595953945</v>
-      </c>
-      <c r="R7" s="2">
-        <f t="shared" ref="R7:Y7" si="6">F32</f>
-        <v>19.255959591887141</v>
-      </c>
-      <c r="S7" s="2">
-        <f t="shared" si="6"/>
-        <v>2.3125784013713306</v>
-      </c>
-      <c r="T7" s="2">
-        <f t="shared" si="6"/>
-        <v>0.65676433051167704</v>
-      </c>
-      <c r="U7" s="2">
-        <f t="shared" si="6"/>
-        <v>42.035678736405572</v>
-      </c>
-      <c r="V7" s="2">
-        <f t="shared" si="6"/>
-        <v>0.16234546040925302</v>
-      </c>
-      <c r="W7" s="2">
-        <f t="shared" si="6"/>
-        <v>4097.9695449810424</v>
-      </c>
-      <c r="X7" s="2">
-        <f t="shared" si="6"/>
-        <v>0.46538329618131491</v>
-      </c>
-      <c r="Y7" s="2">
-        <f t="shared" si="6"/>
-        <v>123.31900595953945</v>
-      </c>
+      <c r="Q7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1107,42 +960,17 @@
       <c r="P8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="2">
-        <f>E37</f>
-        <v>468.65575758667728</v>
-      </c>
-      <c r="R8" s="2">
-        <f t="shared" ref="R8:Y8" si="7">F37</f>
-        <v>2.4736787942808065</v>
-      </c>
-      <c r="S8" s="2">
-        <f t="shared" si="7"/>
-        <v>1.1126627568663274</v>
-      </c>
-      <c r="T8" s="2">
-        <f t="shared" si="7"/>
-        <v>0.72174252451938636</v>
-      </c>
-      <c r="U8" s="2">
-        <f t="shared" si="7"/>
-        <v>56.785760173723283</v>
-      </c>
-      <c r="V8" s="2">
-        <f t="shared" si="7"/>
-        <v>0.20102344184724555</v>
-      </c>
-      <c r="W8" s="2">
-        <f t="shared" si="7"/>
-        <v>1381.4714481325927</v>
-      </c>
-      <c r="X8" s="2">
-        <f t="shared" si="7"/>
-        <v>0.15849516802335994</v>
-      </c>
-      <c r="Y8" s="2">
-        <f t="shared" si="7"/>
-        <v>468.65575758667728</v>
-      </c>
+      <c r="Q8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1190,42 +1018,17 @@
       <c r="P9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q9" s="2">
-        <f>E42</f>
-        <v>214.56234704803299</v>
-      </c>
-      <c r="R9" s="2">
-        <f t="shared" ref="R9:Y9" si="8">F42</f>
-        <v>0.19511963118038433</v>
-      </c>
-      <c r="S9" s="2">
-        <f t="shared" si="8"/>
-        <v>0.42086108406590933</v>
-      </c>
-      <c r="T9" s="2">
-        <f t="shared" si="8"/>
-        <v>0.34053949247954435</v>
-      </c>
-      <c r="U9" s="2">
-        <f t="shared" si="8"/>
-        <v>1.3875085341573137</v>
-      </c>
-      <c r="V9" s="2">
-        <f t="shared" si="8"/>
-        <v>0.13956685494792001</v>
-      </c>
-      <c r="W9" s="2">
-        <f t="shared" si="8"/>
-        <v>102.56221892545916</v>
-      </c>
-      <c r="X9" s="2">
-        <f t="shared" si="8"/>
-        <v>0.59306660050556126</v>
-      </c>
-      <c r="Y9" s="2">
-        <f t="shared" si="8"/>
-        <v>214.56234704803299</v>
-      </c>
+      <c r="Q9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -1239,35 +1042,35 @@
         <v>214.71557153383665</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ref="F10:M10" si="9">AVERAGE(F7:F9)</f>
+        <f t="shared" ref="F10:M10" si="1">AVERAGE(F7:F9)</f>
         <v>0.28003990870250622</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.47263579594587402</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.36327940323608904</v>
       </c>
       <c r="I10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>1.4575641553764784</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.16783744476480314</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>119.54853129157205</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.32006144316351964</v>
       </c>
       <c r="M10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>214.71557153383665</v>
       </c>
       <c r="O10" s="2" t="s">
@@ -1276,42 +1079,17 @@
       <c r="P10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q10" s="2">
-        <f>E48</f>
-        <v>110.55067152523561</v>
-      </c>
-      <c r="R10" s="2">
-        <f t="shared" ref="R10:Y10" si="10">F48</f>
-        <v>19.601298014287153</v>
-      </c>
-      <c r="S10" s="2">
-        <f t="shared" si="10"/>
-        <v>2.4346371370662943</v>
-      </c>
-      <c r="T10" s="2">
-        <f t="shared" si="10"/>
-        <v>0.67346027544119558</v>
-      </c>
-      <c r="U10" s="2">
-        <f t="shared" si="10"/>
-        <v>90.755147422459032</v>
-      </c>
-      <c r="V10" s="2">
-        <f t="shared" si="10"/>
-        <v>0.2969391297790413</v>
-      </c>
-      <c r="W10" s="2">
-        <f t="shared" si="10"/>
-        <v>4159.8814953051915</v>
-      </c>
-      <c r="X10" s="2">
-        <f t="shared" si="10"/>
-        <v>-0.96489455523585466</v>
-      </c>
-      <c r="Y10" s="2">
-        <f t="shared" si="10"/>
-        <v>110.55067152523561</v>
-      </c>
+      <c r="Q10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
@@ -1333,42 +1111,17 @@
       <c r="P11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="2">
-        <f>E53</f>
-        <v>409.36008549481835</v>
-      </c>
-      <c r="R11" s="2">
-        <f t="shared" ref="R11:Y11" si="11">F53</f>
-        <v>1.2360592700689201</v>
-      </c>
-      <c r="S11" s="2">
-        <f t="shared" si="11"/>
-        <v>0.81235632134818925</v>
-      </c>
-      <c r="T11" s="2">
-        <f t="shared" si="11"/>
-        <v>0.62946672376015966</v>
-      </c>
-      <c r="U11" s="2">
-        <f t="shared" si="11"/>
-        <v>40.860767147659523</v>
-      </c>
-      <c r="V11" s="2">
-        <f t="shared" si="11"/>
-        <v>0.14460932422411651</v>
-      </c>
-      <c r="W11" s="2">
-        <f t="shared" si="11"/>
-        <v>701.65944622449842</v>
-      </c>
-      <c r="X11" s="2">
-        <f t="shared" si="11"/>
-        <v>0.58125767165485231</v>
-      </c>
-      <c r="Y11" s="2">
-        <f t="shared" si="11"/>
-        <v>409.36008549481835</v>
-      </c>
+      <c r="Q11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1416,42 +1169,17 @@
       <c r="P12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q12" s="2">
-        <f>E58</f>
-        <v>191.16977630748298</v>
-      </c>
-      <c r="R12" s="2">
-        <f t="shared" ref="R12:Y12" si="12">F58</f>
-        <v>0.1680766216590838</v>
-      </c>
-      <c r="S12" s="2">
-        <f t="shared" si="12"/>
-        <v>0.38729100354190399</v>
-      </c>
-      <c r="T12" s="2">
-        <f t="shared" si="12"/>
-        <v>0.31463094704877764</v>
-      </c>
-      <c r="U12" s="2">
-        <f t="shared" si="12"/>
-        <v>1.2884826766777995</v>
-      </c>
-      <c r="V12" s="2">
-        <f t="shared" si="12"/>
-        <v>0.12930744277187406</v>
-      </c>
-      <c r="W12" s="2">
-        <f t="shared" si="12"/>
-        <v>83.148670627197063</v>
-      </c>
-      <c r="X12" s="2">
-        <f t="shared" si="12"/>
-        <v>0.64584397361352364</v>
-      </c>
-      <c r="Y12" s="2">
-        <f t="shared" si="12"/>
-        <v>191.16977630748298</v>
-      </c>
+      <c r="Q12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1499,42 +1227,17 @@
       <c r="P13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q13" s="2">
-        <f>E64</f>
-        <v>123.6285751399338</v>
-      </c>
-      <c r="R13" s="2">
-        <f t="shared" ref="R13:Y13" si="13">F64</f>
-        <v>18.76326816571013</v>
-      </c>
-      <c r="S13" s="2">
-        <f t="shared" si="13"/>
-        <v>2.2872552117043981</v>
-      </c>
-      <c r="T13" s="2">
-        <f t="shared" si="13"/>
-        <v>0.66365564267318566</v>
-      </c>
-      <c r="U13" s="2">
-        <f t="shared" si="13"/>
-        <v>39.0803037505598</v>
-      </c>
-      <c r="V13" s="2">
-        <f t="shared" si="13"/>
-        <v>0.10004115057687993</v>
-      </c>
-      <c r="W13" s="2">
-        <f t="shared" si="13"/>
-        <v>3991.3215389198695</v>
-      </c>
-      <c r="X13" s="2">
-        <f t="shared" si="13"/>
-        <v>0.59871293012017013</v>
-      </c>
-      <c r="Y13" s="2">
-        <f t="shared" si="13"/>
-        <v>123.6285751399338</v>
-      </c>
+      <c r="Q13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -1630,35 +1333,35 @@
         <v>107.54472776739135</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" ref="F16:M16" si="14">AVERAGE(F12:F15)</f>
+        <f t="shared" ref="F16:M16" si="2">AVERAGE(F12:F15)</f>
         <v>18.990594140551121</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>2.2569177029583769</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>0.5560004238669457</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>21.771239342500404</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>9.2366635485227333E-2</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>4043.3728961514335</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>0.68212620583395711</v>
       </c>
       <c r="M16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>107.54472776739135</v>
       </c>
     </row>
@@ -1812,31 +1515,31 @@
         <v>294.83922401114938</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ref="F21:L21" si="15">AVERAGE(F18:F20)</f>
+        <f t="shared" ref="F21:L21" si="3">AVERAGE(F18:F20)</f>
         <v>0.40268563150320075</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="3"/>
         <v>0.5099631232466697</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="3"/>
         <v>0.42850104887735235</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="3"/>
         <v>23.365672473199567</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="3"/>
         <v>8.8298729960432434E-2</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="3"/>
         <v>244.90157111474659</v>
       </c>
       <c r="L21" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="3"/>
         <v>0.86444195165420956</v>
       </c>
       <c r="M21" s="3">
@@ -1994,27 +1697,27 @@
         <v>239.838588937032</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" ref="F26:M26" si="16">AVERAGE(F23:F25)</f>
+        <f t="shared" ref="F26:M26" si="4">AVERAGE(F23:F25)</f>
         <v>0.54725963738798844</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>0.605114766793307</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>0.45106143856569797</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>1.7850433305725264</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>0.23020885798238935</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>196.60128855458296</v>
       </c>
       <c r="L26" s="3">
@@ -2022,7 +1725,7 @@
         <v>-0.47296155363793796</v>
       </c>
       <c r="M26" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>239.838588937032</v>
       </c>
     </row>
@@ -2217,35 +1920,35 @@
         <v>123.31900595953945</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" ref="F32:M32" si="17">AVERAGE(F28:F31)</f>
+        <f t="shared" ref="F32:M32" si="5">AVERAGE(F28:F31)</f>
         <v>19.255959591887141</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>2.3125784013713306</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>0.65676433051167704</v>
       </c>
       <c r="I32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>42.035678736405572</v>
       </c>
       <c r="J32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>0.16234546040925302</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>4097.9695449810424</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>0.46538329618131491</v>
       </c>
       <c r="M32" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>123.31900595953945</v>
       </c>
     </row>
@@ -2399,35 +2102,35 @@
         <v>468.65575758667728</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ref="F37:M37" si="18">AVERAGE(F34:F36)</f>
+        <f t="shared" ref="F37:M37" si="6">AVERAGE(F34:F36)</f>
         <v>2.4736787942808065</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="6"/>
         <v>1.1126627568663274</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="6"/>
         <v>0.72174252451938636</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="6"/>
         <v>56.785760173723283</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="6"/>
         <v>0.20102344184724555</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="6"/>
         <v>1381.4714481325927</v>
       </c>
       <c r="L37" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="6"/>
         <v>0.15849516802335994</v>
       </c>
       <c r="M37" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="6"/>
         <v>468.65575758667728</v>
       </c>
     </row>
@@ -2581,35 +2284,35 @@
         <v>214.56234704803299</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" ref="F42:M42" si="19">AVERAGE(F39:F41)</f>
+        <f t="shared" ref="F42:M42" si="7">AVERAGE(F39:F41)</f>
         <v>0.19511963118038433</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>0.42086108406590933</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>0.34053949247954435</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>1.3875085341573137</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>0.13956685494792001</v>
       </c>
       <c r="K42" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>102.56221892545916</v>
       </c>
       <c r="L42" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>0.59306660050556126</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>214.56234704803299</v>
       </c>
     </row>
@@ -2804,35 +2507,35 @@
         <v>110.55067152523561</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" ref="F48:M48" si="20">AVERAGE(F44:F47)</f>
+        <f t="shared" ref="F48:M48" si="8">AVERAGE(F44:F47)</f>
         <v>19.601298014287153</v>
       </c>
       <c r="G48" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>2.4346371370662943</v>
       </c>
       <c r="H48" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>0.67346027544119558</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>90.755147422459032</v>
       </c>
       <c r="J48" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>0.2969391297790413</v>
       </c>
       <c r="K48" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>4159.8814953051915</v>
       </c>
       <c r="L48" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>-0.96489455523585466</v>
       </c>
       <c r="M48" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>110.55067152523561</v>
       </c>
     </row>
@@ -2986,35 +2689,35 @@
         <v>409.36008549481835</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" ref="F53:M53" si="21">AVERAGE(F50:F52)</f>
+        <f t="shared" ref="F53:M53" si="9">AVERAGE(F50:F52)</f>
         <v>1.2360592700689201</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>0.81235632134818925</v>
       </c>
       <c r="H53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>0.62946672376015966</v>
       </c>
       <c r="I53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>40.860767147659523</v>
       </c>
       <c r="J53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>0.14460932422411651</v>
       </c>
       <c r="K53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>701.65944622449842</v>
       </c>
       <c r="L53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>0.58125767165485231</v>
       </c>
       <c r="M53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>409.36008549481835</v>
       </c>
     </row>
@@ -3168,35 +2871,35 @@
         <v>191.16977630748298</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" ref="F58:M58" si="22">AVERAGE(F55:F57)</f>
+        <f t="shared" ref="F58:M58" si="10">AVERAGE(F55:F57)</f>
         <v>0.1680766216590838</v>
       </c>
       <c r="G58" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>0.38729100354190399</v>
       </c>
       <c r="H58" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>0.31463094704877764</v>
       </c>
       <c r="I58" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>1.2884826766777995</v>
       </c>
       <c r="J58" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>0.12930744277187406</v>
       </c>
       <c r="K58" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>83.148670627197063</v>
       </c>
       <c r="L58" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>0.64584397361352364</v>
       </c>
       <c r="M58" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>191.16977630748298</v>
       </c>
     </row>
@@ -3391,45 +3094,40 @@
         <v>123.6285751399338</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" ref="F64:M64" si="23">AVERAGE(F60:F63)</f>
+        <f t="shared" ref="F64:M64" si="11">AVERAGE(F60:F63)</f>
         <v>18.76326816571013</v>
       </c>
       <c r="G64" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>2.2872552117043981</v>
       </c>
       <c r="H64" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>0.66365564267318566</v>
       </c>
       <c r="I64" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>39.0803037505598</v>
       </c>
       <c r="J64" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>0.10004115057687993</v>
       </c>
       <c r="K64" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>3991.3215389198695</v>
       </c>
       <c r="L64" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>0.59871293012017013</v>
       </c>
       <c r="M64" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>123.6285751399338</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A58:D58"/>
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A32:D32"/>
@@ -3437,6 +3135,11 @@
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A58:D58"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>